<commit_message>
Corrected PN in BOM
</commit_message>
<xml_diff>
--- a/fabrication_outputs/iCE40hxk4_dev_board.xlsx
+++ b/fabrication_outputs/iCE40hxk4_dev_board.xlsx
@@ -1885,12 +1885,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
-    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="0.00_ "/>
   </numFmts>
   <fonts count="27">
     <font>
@@ -1940,30 +1940,47 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1978,30 +1995,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2022,26 +2023,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2054,22 +2047,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2083,9 +2061,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2136,13 +2136,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2160,127 +2286,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2292,13 +2304,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2310,13 +2316,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2327,15 +2327,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -2398,6 +2389,15 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4"/>
       </bottom>
@@ -2407,8 +2407,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2432,19 +2432,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2453,116 +2447,122 @@
     <xf numFmtId="0" fontId="14" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -2571,7 +2571,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2586,13 +2586,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3052,7 +3052,7 @@
   <sheetPr/>
   <dimension ref="A1:AM167"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="B53" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="B45" workbookViewId="0">
       <selection activeCell="F88" sqref="F88"/>
     </sheetView>
   </sheetViews>
@@ -3179,7 +3179,7 @@
       <c r="AL5" s="14"/>
       <c r="AM5" s="14"/>
     </row>
-    <row r="6" ht="26.7" spans="1:39">
+    <row r="6" spans="1:39">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -8761,7 +8761,7 @@
         <v>202</v>
       </c>
       <c r="F84" t="s">
-        <v>102</v>
+        <v>203</v>
       </c>
       <c r="G84">
         <f>BoardQty*1</f>
@@ -13912,7 +13912,7 @@
       <formula>H7</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F7:F86">
+  <conditionalFormatting sqref="F7:F84;F85:F86">
     <cfRule type="expression" dxfId="1" priority="2" stopIfTrue="1">
       <formula>COUNTIF($F$7:$F$86,F7)&gt;1</formula>
     </cfRule>
@@ -14160,7 +14160,7 @@
     <hyperlink ref="AA85" r:id="rId193" display="Link"/>
     <hyperlink ref="AG85" r:id="rId194" display="Link"/>
   </hyperlinks>
-  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.511111111111111" footer="0.511111111111111"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.510416666666667" footer="0.510416666666667"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
   <legacyDrawing r:id="rId2"/>
@@ -14183,7 +14183,7 @@
         <v>1</v>
       </c>
       <c r="E14">
-        <f>COUNTIF($C$14:$C$18,C14)</f>
+        <f t="shared" ref="E14:E18" si="0">COUNTIF($C$14:$C$18,C14)</f>
         <v>2</v>
       </c>
     </row>
@@ -14191,9 +14191,8 @@
       <c r="C15">
         <v>2</v>
       </c>
-      <c r="D15"/>
       <c r="E15">
-        <f>COUNTIF($C$14:$C$18,C15)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -14201,9 +14200,8 @@
       <c r="C16">
         <v>3</v>
       </c>
-      <c r="D16"/>
       <c r="E16">
-        <f>COUNTIF($C$14:$C$18,C16)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -14212,7 +14210,7 @@
         <v>4</v>
       </c>
       <c r="E17">
-        <f>COUNTIF($C$14:$C$18,C17)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -14221,7 +14219,7 @@
         <v>1</v>
       </c>
       <c r="E18">
-        <f>COUNTIF($C$14:$C$18,C18)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
     </row>

</xml_diff>